<commit_message>
Fjerner TRA - Jonathans Kladder
</commit_message>
<xml_diff>
--- a/Kladder/TRA - Jonathans kladder/Shipping/Freight/Vessels in port.xlsx
+++ b/Kladder/TRA - Jonathans kladder/Shipping/Freight/Vessels in port.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/GitHub/Bachelor_Git/TRA - Jonathans kladder/Shipping/Freight/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/GitHub/Bachelor_Git/Kladder/TRA - Jonathans kladder/Shipping/Freight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6240A8D2-3022-0D42-8B74-CF66F852690F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1737B9DD-5083-644E-A4F5-297D90545146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="55">
   <si>
     <t>Vessels in main ports by type and size of vessels (based on inwards declarations) - quarterly data [MAR_TF_QM__custom_2368560]</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Sum of Freight Ships</t>
   </si>
 </sst>
 </file>
@@ -214,27 +217,32 @@
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -308,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -356,6 +364,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -363,10 +376,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,22 +769,22 @@
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1052,13 +1061,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1070,14 +1079,15 @@
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="19" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -1085,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1093,8 +1103,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1102,7 +1112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1110,7 +1120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1118,12 +1128,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1141,11 +1151,14 @@
       <c r="G9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>47</v>
       </c>
@@ -1167,8 +1180,9 @@
       <c r="G10" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -1190,8 +1204,12 @@
       <c r="G11" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="8">
+        <f>SUM(D11:F11)</f>
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1213,8 +1231,12 @@
       <c r="G12" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="8">
+        <f t="shared" ref="H12:H22" si="0">SUM(D12:F12)</f>
+        <v>3637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1236,8 +1258,12 @@
       <c r="G13" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="8">
+        <f t="shared" si="0"/>
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
@@ -1259,12 +1285,16 @@
       <c r="G14" s="9">
         <v>16</v>
       </c>
-      <c r="H14" s="21">
-        <f>AVERAGE(C11:C14)</f>
-        <v>26799.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
+        <v>3873</v>
+      </c>
+      <c r="I14" s="19">
+        <f>SUM(H11:H14)</f>
+        <v>14825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1286,8 +1316,12 @@
       <c r="G15" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>3446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -1309,8 +1343,12 @@
       <c r="G16" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="8">
+        <f t="shared" si="0"/>
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1332,8 +1370,12 @@
       <c r="G17" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="8">
+        <f t="shared" si="0"/>
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -1355,12 +1397,16 @@
       <c r="G18" s="9">
         <v>9</v>
       </c>
-      <c r="H18" s="21">
-        <f>AVERAGE(C15:C18)</f>
-        <v>27861.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="8">
+        <f t="shared" si="0"/>
+        <v>3451</v>
+      </c>
+      <c r="I18" s="19">
+        <f>SUM(H15:H18)</f>
+        <v>14009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1382,8 +1428,12 @@
       <c r="G19" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>29</v>
       </c>
@@ -1405,8 +1455,12 @@
       <c r="G20" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="8">
+        <f t="shared" si="0"/>
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>29</v>
       </c>
@@ -1428,8 +1482,12 @@
       <c r="G21" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="8">
+        <f t="shared" si="0"/>
+        <v>2628</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
@@ -1451,17 +1509,21 @@
       <c r="G22" s="9">
         <v>3</v>
       </c>
-      <c r="H22" s="21">
-        <f>AVERAGE(C19:C22)</f>
-        <v>27593.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="8">
+        <f t="shared" si="0"/>
+        <v>2652</v>
+      </c>
+      <c r="I22" s="19">
+        <f>SUM(H19:H22)</f>
+        <v>10679</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>